<commit_message>
&& git push github main
</commit_message>
<xml_diff>
--- a/ranks/BUPT 2024 Winter Welcome Wagon #1.xlsx
+++ b/ranks/BUPT 2024 Winter Welcome Wagon #1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K35"/>
+  <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -510,12 +510,12 @@
       </c>
       <c r="F2" s="1" t="inlineStr">
         <is>
-          <t>30 / 74</t>
+          <t>31 / 77</t>
         </is>
       </c>
       <c r="G2" s="1" t="inlineStr">
         <is>
-          <t>31 / 38</t>
+          <t>32 / 39</t>
         </is>
       </c>
       <c r="H2" s="1" t="inlineStr">
@@ -530,7 +530,7 @@
       </c>
       <c r="J2" s="1" t="inlineStr">
         <is>
-          <t>3 / 13</t>
+          <t>3 / 15</t>
         </is>
       </c>
       <c r="K2" s="1" t="inlineStr">
@@ -1321,7 +1321,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Asrit (安澍)</t>
+          <t>Sherlocked_hzoi (王若竹)</t>
         </is>
       </c>
       <c r="D23" t="n">
@@ -1329,22 +1329,26 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>106  1:46:06</t>
+          <t>68  1:08:35</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>0:27:05  (-2)</t>
+          <t>0:10:29  (-2)</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>0:39:01</t>
+          <t>0:18:06</t>
         </is>
       </c>
       <c r="H23" t="inlineStr"/>
       <c r="I23" t="inlineStr"/>
-      <c r="J23" t="inlineStr"/>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>(-2)</t>
+        </is>
+      </c>
       <c r="K23" t="inlineStr"/>
     </row>
     <row r="24">
@@ -1356,7 +1360,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>nonname55 (马骐荣)</t>
+          <t>Asrit (安澍)</t>
         </is>
       </c>
       <c r="D24" t="n">
@@ -1364,24 +1368,20 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>200  3:20:21</t>
+          <t>106  1:46:06</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>0:49:30  (-4)</t>
+          <t>0:27:05  (-2)</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>1:10:51</t>
-        </is>
-      </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t>(-5)</t>
-        </is>
-      </c>
+          <t>0:39:01</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr"/>
       <c r="I24" t="inlineStr"/>
       <c r="J24" t="inlineStr"/>
       <c r="K24" t="inlineStr"/>
@@ -1395,7 +1395,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>daisyandgalsang (田苗)</t>
+          <t>nonname55 (马骐荣)</t>
         </is>
       </c>
       <c r="D25" t="n">
@@ -1403,20 +1403,24 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>213  3:33:14</t>
+          <t>200  3:20:21</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>1:02:10  (-2)</t>
+          <t>0:49:30  (-4)</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>1:51:04</t>
-        </is>
-      </c>
-      <c r="H25" t="inlineStr"/>
+          <t>1:10:51</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>(-5)</t>
+        </is>
+      </c>
       <c r="I25" t="inlineStr"/>
       <c r="J25" t="inlineStr"/>
       <c r="K25" t="inlineStr"/>
@@ -1430,7 +1434,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>superzzc (张智成)</t>
+          <t>daisyandgalsang (田苗)</t>
         </is>
       </c>
       <c r="D26" t="n">
@@ -1438,20 +1442,20 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>235  3:55:14</t>
-        </is>
-      </c>
-      <c r="F26" t="inlineStr"/>
+          <t>213  3:33:14</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>1:02:10  (-2)</t>
+        </is>
+      </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>1:09:53</t>
-        </is>
-      </c>
-      <c r="H26" t="inlineStr">
-        <is>
-          <t>2:45:21</t>
-        </is>
-      </c>
+          <t>1:51:04</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr"/>
       <c r="I26" t="inlineStr"/>
       <c r="J26" t="inlineStr"/>
       <c r="K26" t="inlineStr"/>
@@ -1465,7 +1469,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>xwang603 (王鑫)</t>
+          <t>superzzc (张智成)</t>
         </is>
       </c>
       <c r="D27" t="n">
@@ -1473,20 +1477,20 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>285  4:45:03</t>
-        </is>
-      </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>1:16:35  (-5)</t>
-        </is>
-      </c>
+          <t>235  3:55:14</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr"/>
       <c r="G27" t="inlineStr">
         <is>
-          <t>1:48:28</t>
-        </is>
-      </c>
-      <c r="H27" t="inlineStr"/>
+          <t>1:09:53</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>2:45:21</t>
+        </is>
+      </c>
       <c r="I27" t="inlineStr"/>
       <c r="J27" t="inlineStr"/>
       <c r="K27" t="inlineStr"/>
@@ -1500,7 +1504,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>scyyy (杨树灿)</t>
+          <t>xwang603 (王鑫)</t>
         </is>
       </c>
       <c r="D28" t="n">
@@ -1508,17 +1512,17 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>292  4:52:10</t>
+          <t>285  4:45:03</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>1:31:52  (-3)</t>
+          <t>1:16:35  (-5)</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>2:20:18</t>
+          <t>1:48:28</t>
         </is>
       </c>
       <c r="H28" t="inlineStr"/>
@@ -1535,7 +1539,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>sunchaser</t>
+          <t>scyyy (杨树灿)</t>
         </is>
       </c>
       <c r="D29" t="n">
@@ -1543,17 +1547,17 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>311  5:11:14</t>
+          <t>292  4:52:10</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>2:46:02</t>
+          <t>1:31:52  (-3)</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>2:25:12</t>
+          <t>2:20:18</t>
         </is>
       </c>
       <c r="H29" t="inlineStr"/>
@@ -1570,7 +1574,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>yidau (赵佳一)</t>
+          <t>sunchaser</t>
         </is>
       </c>
       <c r="D30" t="n">
@@ -1578,26 +1582,22 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>372  6:12:09</t>
+          <t>311  5:11:14</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>1:45:45  (-2)</t>
+          <t>2:46:02</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>3:06:24  (-2)</t>
+          <t>2:25:12</t>
         </is>
       </c>
       <c r="H30" t="inlineStr"/>
       <c r="I30" t="inlineStr"/>
-      <c r="J30" t="inlineStr">
-        <is>
-          <t>(-1)</t>
-        </is>
-      </c>
+      <c r="J30" t="inlineStr"/>
       <c r="K30" t="inlineStr"/>
     </row>
     <row r="31">
@@ -1609,7 +1609,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>YLXS (王智炜)</t>
+          <t>yidau (赵佳一)</t>
         </is>
       </c>
       <c r="D31" t="n">
@@ -1617,22 +1617,26 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>389  6:29:54</t>
+          <t>372  6:12:09</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>2:45:35</t>
+          <t>1:45:45  (-2)</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>3:44:19</t>
+          <t>3:06:24  (-2)</t>
         </is>
       </c>
       <c r="H31" t="inlineStr"/>
       <c r="I31" t="inlineStr"/>
-      <c r="J31" t="inlineStr"/>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>(-1)</t>
+        </is>
+      </c>
       <c r="K31" t="inlineStr"/>
     </row>
     <row r="32">
@@ -1644,7 +1648,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>use_rn_me (李乐扬)</t>
+          <t>YLXS (王智炜)</t>
         </is>
       </c>
       <c r="D32" t="n">
@@ -1652,17 +1656,17 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>394  6:34:27</t>
+          <t>389  6:29:54</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>3:02:22  (-1)</t>
+          <t>2:45:35</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>3:12:05</t>
+          <t>3:44:19</t>
         </is>
       </c>
       <c r="H32" t="inlineStr"/>
@@ -1679,7 +1683,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>wryyyy (王宸宇)</t>
+          <t>use_rn_me (李乐扬)</t>
         </is>
       </c>
       <c r="D33" t="n">
@@ -1687,17 +1691,17 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>427  7:07:06</t>
+          <t>394  6:34:27</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>3:25:09</t>
+          <t>3:02:22  (-1)</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>3:41:57</t>
+          <t>3:12:05</t>
         </is>
       </c>
       <c r="H33" t="inlineStr"/>
@@ -1714,7 +1718,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>neetman (秦维斌)</t>
+          <t>wryyyy (王宸宇)</t>
         </is>
       </c>
       <c r="D34" t="n">
@@ -1722,17 +1726,17 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>463  7:43:34</t>
+          <t>427  7:07:06</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>3:18:29  (-1)</t>
+          <t>3:25:09</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>3:45:05  (-1)</t>
+          <t>3:41:57</t>
         </is>
       </c>
       <c r="H34" t="inlineStr"/>
@@ -1749,23 +1753,58 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>oql (区庆亮)</t>
+          <t>neetman (秦维斌)</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>41  0:41:04</t>
-        </is>
-      </c>
-      <c r="F35" t="inlineStr"/>
-      <c r="G35" t="inlineStr"/>
+          <t>463  7:43:34</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>3:18:29  (-1)</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>3:45:05  (-1)</t>
+        </is>
+      </c>
       <c r="H35" t="inlineStr"/>
       <c r="I35" t="inlineStr"/>
       <c r="J35" t="inlineStr"/>
-      <c r="K35" t="inlineStr">
+      <c r="K35" t="inlineStr"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B36" t="n">
+        <v>33</v>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>oql (区庆亮)</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>1</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>41  0:41:04</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr"/>
+      <c r="G36" t="inlineStr"/>
+      <c r="H36" t="inlineStr"/>
+      <c r="I36" t="inlineStr"/>
+      <c r="J36" t="inlineStr"/>
+      <c r="K36" t="inlineStr">
         <is>
           <t>0:41:04</t>
         </is>

</xml_diff>